<commit_message>
updating RDS files with new cleaning procedure
</commit_message>
<xml_diff>
--- a/Documentation/R Microsim Model - Parameter Dictionary.xlsx
+++ b/Documentation/R Microsim Model - Parameter Dictionary.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="316">
   <si>
     <t>Purpose: Dictionary for policy_simulation() function parameters</t>
   </si>
@@ -977,6 +977,9 @@
   </si>
   <si>
     <t>Proportion of dual receivers in the population</t>
+  </si>
+  <si>
+    <t>Takes precedence over any uptake_* parameter values fed into the model for leave needers</t>
   </si>
 </sst>
 </file>
@@ -1390,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,6 +1719,9 @@
       </c>
       <c r="H16" s="4" t="b">
         <v>0</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">

</xml_diff>